<commit_message>
Started implementing [eb2]. Not finished.
</commit_message>
<xml_diff>
--- a/cond-files/cond_eb1_cue_predictive.xlsx
+++ b/cond-files/cond_eb1_cue_predictive.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\Dropbox\Projects\eb\eb\cond-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egora\Dropbox\Projects\eb\eb\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1FD737-45CF-440E-93E2-F95BF088EE0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7A073A-C7DA-43E9-ACCD-817319EBE93B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="92" yWindow="144" windowWidth="16259" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="14020" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="cond_eb1_c" sheetId="1" r:id="rId1"/>
+    <sheet name="cond" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 

</xml_diff>